<commit_message>
fix bug with students criteria calculations
</commit_message>
<xml_diff>
--- a/src/main/python/test_xlsx_files/exp_data.xlsx
+++ b/src/main/python/test_xlsx_files/exp_data.xlsx
@@ -445,10 +445,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.3451</v>
+        <v>0.03451</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3255</v>
+        <v>0.03255</v>
       </c>
       <c r="C3" t="n">
         <v>0.033</v>
@@ -500,7 +500,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.6338</v>
+        <v>0.06338000000000001</v>
       </c>
       <c r="B8" t="n">
         <v>0.06412</v>

</xml_diff>